<commit_message>
new branch for gulp
</commit_message>
<xml_diff>
--- a/assets/wireframe/Chainz Data structure.xlsx
+++ b/assets/wireframe/Chainz Data structure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="12260" tabRatio="500"/>
+    <workbookView xWindow="5440" yWindow="0" windowWidth="24540" windowHeight="13360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>Users</t>
   </si>
@@ -459,20 +459,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G16"/>
+  <dimension ref="B3:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="3" spans="2:7" ht="15.75" customHeight="1">
+    <row r="3" spans="2:9" ht="15.75" customHeight="1">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="15.75" customHeight="1">
+    <row r="4" spans="2:9" ht="15.75" customHeight="1">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -489,12 +489,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="15.75" customHeight="1">
+    <row r="6" spans="2:9" ht="15.75" customHeight="1">
       <c r="B6" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="15.75" customHeight="1">
+    <row r="7" spans="2:9" ht="15.75" customHeight="1">
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
@@ -513,8 +513,14 @@
       <c r="G7" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" ht="15.75" customHeight="1">
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="15.75" customHeight="1">
       <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
@@ -531,12 +537,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="15.75" customHeight="1">
+    <row r="10" spans="2:9" ht="15.75" customHeight="1">
       <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="15.75" customHeight="1">
+    <row r="11" spans="2:9" ht="15.75" customHeight="1">
       <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
@@ -551,7 +557,7 @@
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="2:7" ht="15.75" customHeight="1">
+    <row r="12" spans="2:9" ht="15.75" customHeight="1">
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
@@ -566,12 +572,12 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="15" spans="2:7" ht="15.75" customHeight="1">
+    <row r="15" spans="2:9" ht="15.75" customHeight="1">
       <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="2:7" ht="15.75" customHeight="1">
+    <row r="16" spans="2:9" ht="15.75" customHeight="1">
       <c r="B16" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
we made a lot of changes in the wrong branch we need to merge
</commit_message>
<xml_diff>
--- a/assets/wireframe/Chainz Data structure.xlsx
+++ b/assets/wireframe/Chainz Data structure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5440" yWindow="0" windowWidth="24540" windowHeight="13360" tabRatio="500"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>Users</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>passwordDigest</t>
-  </si>
-  <si>
-    <t>challengesId</t>
   </si>
   <si>
     <t>active</t>
@@ -462,7 +459,7 @@
   <dimension ref="B3:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -486,12 +483,12 @@
         <v>4</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="15.75" customHeight="1">
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="15.75" customHeight="1">
@@ -502,44 +499,44 @@
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="H7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" t="s">
         <v>19</v>
-      </c>
-      <c r="I7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="15.75" customHeight="1">
       <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="15.75" customHeight="1">
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="15.75" customHeight="1">
@@ -547,48 +544,48 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="2:9" ht="15.75" customHeight="1">
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="15" spans="2:9" ht="15.75" customHeight="1">
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="15.75" customHeight="1">
       <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added relationships for checker model
</commit_message>
<xml_diff>
--- a/assets/wireframe/Chainz Data structure.xlsx
+++ b/assets/wireframe/Chainz Data structure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>Users</t>
   </si>
@@ -63,9 +63,6 @@
     <t>userId</t>
   </si>
   <si>
-    <t>challengeId</t>
-  </si>
-  <si>
     <t>interger</t>
   </si>
   <si>
@@ -85,6 +82,21 @@
   </si>
   <si>
     <t>Challenge</t>
+  </si>
+  <si>
+    <t>challengeId *</t>
+  </si>
+  <si>
+    <t>Tasks_ChallengeId_fkey</t>
+  </si>
+  <si>
+    <t>to Challenges</t>
+  </si>
+  <si>
+    <t>ChallengeId_foreign_idx</t>
+  </si>
+  <si>
+    <t>* foreign keys</t>
   </si>
 </sst>
 </file>
@@ -456,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:I16"/>
+  <dimension ref="B3:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -483,12 +495,18 @@
         <v>4</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="15.75" customHeight="1">
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="15.75" customHeight="1">
@@ -511,10 +529,10 @@
         <v>8</v>
       </c>
       <c r="H7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" t="s">
         <v>18</v>
-      </c>
-      <c r="I7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="15.75" customHeight="1">
@@ -536,7 +554,7 @@
     </row>
     <row r="10" spans="2:9" ht="15.75" customHeight="1">
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="15.75" customHeight="1">
@@ -550,9 +568,14 @@
         <v>13</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="2:9" ht="15.75" customHeight="1">
       <c r="B12" s="1" t="s">
@@ -565,13 +588,13 @@
         <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="15" spans="2:9" ht="15.75" customHeight="1">
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="15.75" customHeight="1">
@@ -579,13 +602,18 @@
         <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>19</v>
+    </row>
+    <row r="18" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G18" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>